<commit_message>
Update the API list and Visual Studio configuration.
</commit_message>
<xml_diff>
--- a/dismapi.xlsx
+++ b/dismapi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dism-reverse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\MouriNaruto\DISMSDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3623A14-8938-4F60-9633-EFBF1FF84250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCF373-FA49-4F41-B6DC-E88931B13EF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10.0.19041.0" sheetId="1" r:id="rId1"/>
@@ -893,7 +893,7 @@
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D98"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="D53" s="14"/>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="14"/>
+      <c r="D71" s="10"/>
       <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>